<commit_message>
added more resumes data
</commit_message>
<xml_diff>
--- a/input_data/resume_extractor_sheet/resume_extractor_input_sheet.xlsx
+++ b/input_data/resume_extractor_sheet/resume_extractor_input_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4408" uniqueCount="1546">
   <si>
     <t xml:space="preserve">File_name</t>
   </si>
@@ -3869,6 +3869,795 @@
   </si>
   <si>
     <t xml:space="preserve">Accenture Solutions Pvt Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NisheethKumar.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N Is H E Et H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nisheethkr7@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teleperformance India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NISHEETH KUMAR BAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teleperformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potunuru_Keerthana.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potnuru Keerthana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pkeerthana580@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTECH SOFTWARE SOLUTions PVT.LTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Not Identified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTECH SOFTWARE SOLUTIONS PVT.LTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRADEEPTHANKAPPAN.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pradeep Thankappan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pradeep.thankappan@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altice Bell Canada Cablevision Capitel Comcast Genzeon Pvt Ltd Infosys Infosys Technologies Ltd Nortel Sharecare (Digital House) Verizon Warner Brothers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharecare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vivek_gupta.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vivek Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023@deoriaprivet.iti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKH Y TEC India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vivekgupta12356@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pragati_Singh.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Praga Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">278@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATC Tire Private Limited TATA Cummins Private Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pragati Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spragati278@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gujarat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATC Tire Private Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinodkumar.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinod.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91-6302816037vinodkumarmerugu.47@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anil Neuro and Trauma center Avidex Info tech E Teams Info Services Pvt Ltd KK Hospital Sigma Software Solutions Pvt Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinodkumarmerugu.47@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma Software Solutions Pvt Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YatheshReddy.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yathesh Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91-9632419733yatheshreddy321@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adrola software technologies India Private Limited Linkedin service private Limited LTIMindtree Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yathesh Kumar Reddy Saddikuti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yatheshreddy321@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Likedin service private Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AasthaThakur_6y_1m_.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astha Thakur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aastha.thakur-659494167@linkedin.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AASTHA THAKUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aasthathakur6868@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SourabhBhagwat.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sourabh Bhagwat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008@deviahilyavishwavidyalaya.ac.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acpl Systems Pvt Ltd Arbor HCL Technologies Ltd. Hitachi Systems Micro Clinic Wipro Infotech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sourabhb445@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BudhadityaDey.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budhaditya Dey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budhaditya.dey25@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJ Mohan and Associates PwC India (AC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShashankKumarTyagi.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shashank Kumar Tyagi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanutg@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accenture Jellyfish Technologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JellyFish Technologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simran.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chughsimran56@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IIFL Orange Mantra Trupp Global Technologies Pvt. Ltd. Zucol Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IIFL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AbhishekPal.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhishek Pal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abhi.rke39@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCL Technologies Hitachi Systems Micro Clinic PVT. LTD. Infini minds PVT LTD InTarvo Technologies Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namrata_Pujari.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namrata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">namratapujari2002@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solapur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namrata Pujari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnitheswariDevi10y_5m.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anitheswari Devi M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anitheswaridevim@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCL Technologies ProFound Infotech Pvt Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANITHESWARI DEVI M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RajeshKumar.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajesh Kushwaha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajeshkushwahauk@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognizant HCL Technologies, Noida HyTech Services Incedo, Gurgaon iYogi, Gurgaon TCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAJESH KUSHWAHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ashish_lagishetty.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashish Lagishetty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ashishlagishetty@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlueStone Jewellery Levis MARKS &amp; SPENCER RAYMOND - MADE TO MEASURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASHISH LAGISHETTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlueStone Jewellery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaskaran_PalSingh.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaskaran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kalra.jaskaranpal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amritsar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognizant Oncehub Tata Consultancy Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaskaran Pal Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chandigarh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oncehub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NiranjanMazumdar.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niranjan Mazumdar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">niranjan.portal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTI Mindtree RabbitMQ Tata Consultancy Services Wipro Technologies Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTI Mindtree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria_Cristina_Polancos.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Cristina Polancos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cristinabalindo@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converged IT On Point Technology, LCC Smartfoxdata Technomancer Workbank Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA CRISTINA POLANCOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHILIPPINES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMARTFOXDATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mariel_Resume.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mariel D. Onting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mariel.onting4@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taguig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardinal Health International Philippines - Healthcare Account Freelancer Telus International Philippines - Retail Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIEL D. ONTING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardinal Health International Philippines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nishidha.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nishidha C Ail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nishidhacail@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amar Infraprojects Emerge Business Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kasaragod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amar Infraprojects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prashanth6y_6m.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prashanth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erramprashanth5684@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fis TCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VipinRaturi.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vipin Raturi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vipinraturi2244@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genpact Hogarth Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hogarth Studios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahantesh.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahantesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mahiifintech@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altus Mindstream Innovation Pvt Ltd Friesian Technologies Private Limited Marvelle Skin Care Pvt Ltd P Venugopalachari Chartered Accountants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mahiifintech@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altus Mindstream Innovation Pvt Ltd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAHULKAMADI.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahul Kamadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rahulkamadi92@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBM, India Predikly Technologies Pvt. Ltd., India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajay_Santhosh_P.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajay Santhosh P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spajay2000@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuticorin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAKSHIN BHARATH GATEWAY TERMINAL JANAKI TRADERS SHIPPING PVT LTD SEAPOL LOGISTICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JANAKI TRADERS SHIPPING PVT LTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PothalaNeelima.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neelima Pothala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neelupothala@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satyaprakash.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satya Prakash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">satyapraks44@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kotak Mahindra Bank Wells Fargo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SATYA PRAKASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yogeshvri.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yogeshvri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yuktigoel829@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haryana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOGESHVRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BindhuMV.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bindhu Mv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bindhumv1398@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapt IQ (Consleague Consulting)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BINDHU MV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapt IQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajasekhar.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajasekhar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajasekhar.python3366@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CapGemini Gallagher Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CapGemini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rambabu.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rambabu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mtpllram@outlook.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accenture Bank of America, Retirement services SLK Software Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VarshaNaC.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varsha Na C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nac.varsha@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neyveli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IndujapriyaB.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indujapriya B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indujapriya2001@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pollachi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaratLane Trading Pvt Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vipin_yadav_cv.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vipin Yadav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vipinmardanpur@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samvdhana Motherson internation limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virendra_kirar.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viresh Kirar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">virendrakirarbamori@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talegaon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KSPG Automotive takeve Pune Mahindra &amp; Mahindra Ltd chakan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIRENDRA KIRAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahindra &amp; Mahindra Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinay_Kumar_Rauniyar.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinay Rauniyar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vinayrauniyar924@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nifco India Pvt. Ltd PPAP Automotive Pvt. Ltd Sellowrap EPP India Pvt. Ltd Yazaki India Pvt. Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinay Kumar Rauniyar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nifco India Pvt. Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BnarenderRao.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. Narender Rao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naren8487@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognizant Technology Solutions India Private Limited Data Monitoring Venture/Global Data Deloitte Touch Tohmatsu India LLP Deloitte US India Offices Jp Morgan Services India Pvt Ltd Thomson Reuters Wells Fargo International Solutions Private Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wells Fargo International Solutions Private Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRI-USHA.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sriusharani Sudarshanam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sriushasudarshanam@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUDARSHANAM SRI USHA RANI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DigiTeleNetworks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiskaHernandez.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giska Hernandez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gigipiahernandez03@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognizant Softvision - Manila Denso Ten Solutions Philippines Inc. DTN Manila Nowcom Global Solutions LLC Reed Elsevier Shared Services Inc. Philippines Verifone Global Development Center Inc. Philippines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognizant Softvision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ArchanaKhade.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archana Rajendra Khade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">archana.patil84@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cybage Dire Straits Consulting Infosys Ltd Systime Global solutions TechProcess Solutions Pvt Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cybage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DiwakarGupta.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diwakar Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diwakar-gupta-8013b5179@linkedin.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PwC USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diwakar9525@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PwC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RITWIKGUHATHAKURTA.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ritwik Guha Thakurta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ritwikguhathakurta@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Bank of India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padmashree_S.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padmashree S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pshree984@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10kinfo Data Solutions Pvt Ltd Etech IT Solutions (Previously MA IT Solutions) Mekhalyn Consulting (Previously Topsys Solutions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etech IT Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorraine_Ardiente.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorraine Ardiente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ardientelorraine@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xtreme Offshores Outsourcing Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xtreme Offshores Outsourcing Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEHASINGH.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neha Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singh.neha006@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accenture Solutions Private Limited Global Market Insights Hindustan Petroleum Private Limited Ingenious e-Brain Solutions Private Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AmanArora.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aman Arora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa.arora.1996@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon eClerx Intelegencia Analytics Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclerx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJAYSARATHSUBRAMANI.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajay Sarath Subramani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajaysarath.psmani@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aristocrat Interactive (Pariplay India Private Limited) Lion Bridge Technologies Pariplay India Private Limited Scientific Games Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aristocrat Interactive</t>
   </si>
 </sst>
 </file>
@@ -3881,7 +4670,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3958,6 +4747,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF262626"/>
+      <name val="aakar"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1D1D1D"/>
       <name val="aakar"/>
       <family val="0"/>
       <charset val="1"/>
@@ -4069,7 +4865,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4147,6 +4943,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4286,7 +5086,7 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF277E3E"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF1D1D1D"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -4301,17 +5101,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U238"/>
+  <dimension ref="A1:U287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I108" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J130" activeCellId="0" sqref="J130"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F219" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V19" activeCellId="0" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="42.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.46"/>
@@ -12115,7 +12915,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>665</v>
       </c>
@@ -19439,6 +20239,3167 @@
         <v>35</v>
       </c>
       <c r="U238" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B239" s="5" t="n">
+        <v>5948500</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D239" s="5" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E239" s="5" t="n">
+        <v>8563966764</v>
+      </c>
+      <c r="F239" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G239" s="5" t="n">
+        <v>28.9</v>
+      </c>
+      <c r="H239" s="5" t="s">
+        <v>1286</v>
+      </c>
+      <c r="I239" s="5" t="s">
+        <v>1287</v>
+      </c>
+      <c r="J239" s="5" t="s">
+        <v>1285</v>
+      </c>
+      <c r="K239" s="5" t="n">
+        <v>8563966764</v>
+      </c>
+      <c r="L239" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M239" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N239" s="5" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="O239" s="5" t="s">
+        <v>1288</v>
+      </c>
+      <c r="P239" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q239" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R239" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S239" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T239" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U239" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B240" s="5" t="n">
+        <v>5949327</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D240" s="5" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E240" s="5" t="n">
+        <v>6382837356</v>
+      </c>
+      <c r="F240" s="5"/>
+      <c r="G240" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="H240" s="5" t="s">
+        <v>1292</v>
+      </c>
+      <c r="I240" s="5" t="s">
+        <v>1290</v>
+      </c>
+      <c r="J240" s="5" t="s">
+        <v>1291</v>
+      </c>
+      <c r="K240" s="5" t="n">
+        <v>6382837356</v>
+      </c>
+      <c r="L240" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M240" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N240" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O240" s="5" t="s">
+        <v>1294</v>
+      </c>
+      <c r="P240" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q240" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R240" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S240" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T240" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U240" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B241" s="5" t="n">
+        <v>5949796</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D241" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E241" s="5" t="n">
+        <v>8056286774</v>
+      </c>
+      <c r="F241" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G241" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="H241" s="5" t="s">
+        <v>1298</v>
+      </c>
+      <c r="I241" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="J241" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="K241" s="5" t="n">
+        <v>8056286774</v>
+      </c>
+      <c r="L241" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M241" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N241" s="5" t="n">
+        <v>27.8</v>
+      </c>
+      <c r="O241" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="P241" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q241" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R241" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S241" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T241" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U241" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B242" s="5" t="n">
+        <v>5947245</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D242" s="5" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E242" s="5" t="n">
+        <v>8651735805</v>
+      </c>
+      <c r="F242" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G242" s="5" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H242" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="I242" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="J242" s="5" t="s">
+        <v>1304</v>
+      </c>
+      <c r="K242" s="5" t="n">
+        <v>8651735805</v>
+      </c>
+      <c r="L242" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="M242" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N242" s="5" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="O242" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="P242" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q242" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R242" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S242" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T242" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U242" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B243" s="19" t="n">
+        <v>5947355</v>
+      </c>
+      <c r="C243" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D243" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E243" s="5" t="n">
+        <v>6388545076</v>
+      </c>
+      <c r="F243" s="5"/>
+      <c r="G243" s="5" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H243" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="I243" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="J243" s="5" t="s">
+        <v>1310</v>
+      </c>
+      <c r="K243" s="5" t="n">
+        <v>6388545076</v>
+      </c>
+      <c r="L243" s="5" t="s">
+        <v>1311</v>
+      </c>
+      <c r="M243" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N243" s="5" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="O243" s="5" t="s">
+        <v>1312</v>
+      </c>
+      <c r="P243" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q243" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R243" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S243" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T243" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U243" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B244" s="5" t="n">
+        <v>5947667</v>
+      </c>
+      <c r="C244" s="5" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D244" s="5" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E244" s="5" t="n">
+        <v>6302816037</v>
+      </c>
+      <c r="F244" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G244" s="5" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="H244" s="5" t="s">
+        <v>1316</v>
+      </c>
+      <c r="I244" s="5" t="s">
+        <v>1314</v>
+      </c>
+      <c r="J244" s="5" t="s">
+        <v>1317</v>
+      </c>
+      <c r="K244" s="5" t="n">
+        <v>6302816037</v>
+      </c>
+      <c r="L244" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M244" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N244" s="5" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="O244" s="5" t="s">
+        <v>1318</v>
+      </c>
+      <c r="P244" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q244" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R244" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S244" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T244" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U244" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B245" s="5" t="n">
+        <v>5947821</v>
+      </c>
+      <c r="C245" s="5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D245" s="5" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E245" s="5" t="n">
+        <v>9632419733</v>
+      </c>
+      <c r="F245" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G245" s="5" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="H245" s="5" t="s">
+        <v>1322</v>
+      </c>
+      <c r="I245" s="5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="J245" s="5" t="s">
+        <v>1324</v>
+      </c>
+      <c r="K245" s="5" t="n">
+        <v>9632419733</v>
+      </c>
+      <c r="L245" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M245" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N245" s="5" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="O245" s="5" t="s">
+        <v>1325</v>
+      </c>
+      <c r="P245" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q245" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R245" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S245" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T245" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U245" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B246" s="5" t="n">
+        <v>5948628</v>
+      </c>
+      <c r="C246" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D246" s="5" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E246" s="5" t="n">
+        <v>9634702275</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G246" s="5" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="H246" s="5"/>
+      <c r="I246" s="5" t="s">
+        <v>1329</v>
+      </c>
+      <c r="J246" s="5" t="s">
+        <v>1330</v>
+      </c>
+      <c r="K246" s="5" t="n">
+        <v>9634702275</v>
+      </c>
+      <c r="L246" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M246" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N246" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O246" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="P246" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q246" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R246" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S246" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T246" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U246" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B247" s="5" t="n">
+        <v>5948659</v>
+      </c>
+      <c r="C247" s="5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D247" s="5" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E247" s="5" t="n">
+        <v>7838974143</v>
+      </c>
+      <c r="F247" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G247" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H247" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="I247" s="5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="J247" s="5" t="s">
+        <v>1335</v>
+      </c>
+      <c r="K247" s="5" t="n">
+        <v>7838974143</v>
+      </c>
+      <c r="L247" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="M247" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N247" s="5" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="O247" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="P247" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q247" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R247" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S247" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T247" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U247" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B248" s="5" t="n">
+        <v>5947360</v>
+      </c>
+      <c r="C248" s="5" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D248" s="5" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E248" s="5" t="n">
+        <v>11802163</v>
+      </c>
+      <c r="F248" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G248" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="H248" s="5" t="s">
+        <v>1339</v>
+      </c>
+      <c r="I248" s="5" t="s">
+        <v>1337</v>
+      </c>
+      <c r="J248" s="5" t="s">
+        <v>1338</v>
+      </c>
+      <c r="K248" s="5" t="n">
+        <v>9007789112</v>
+      </c>
+      <c r="L248" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="M248" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N248" s="5" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="O248" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="P248" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q248" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R248" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S248" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T248" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U248" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B249" s="5" t="n">
+        <v>5947676</v>
+      </c>
+      <c r="C249" s="5" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D249" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E249" s="5" t="n">
+        <v>10485124</v>
+      </c>
+      <c r="F249" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G249" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="H249" s="5" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I249" s="5" t="s">
+        <v>1341</v>
+      </c>
+      <c r="J249" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K249" s="5" t="n">
+        <v>9901428260</v>
+      </c>
+      <c r="L249" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="M249" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N249" s="5" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="O249" s="5" t="s">
+        <v>1344</v>
+      </c>
+      <c r="P249" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q249" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R249" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S249" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T249" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U249" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B250" s="5" t="n">
+        <v>5948109</v>
+      </c>
+      <c r="C250" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D250" s="5" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E250" s="5" t="n">
+        <v>616175199</v>
+      </c>
+      <c r="F250" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="G250" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H250" s="5" t="s">
+        <v>1348</v>
+      </c>
+      <c r="I250" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="J250" s="5" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K250" s="5" t="n">
+        <v>8168869717</v>
+      </c>
+      <c r="L250" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="M250" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N250" s="5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O250" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="P250" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q250" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R250" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S250" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T250" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U250" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="1" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B251" s="5" t="n">
+        <v>5949397</v>
+      </c>
+      <c r="C251" s="5" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D251" s="5" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E251" s="5" t="n">
+        <v>91094406</v>
+      </c>
+      <c r="F251" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G251" s="5" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H251" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I251" s="5" t="s">
+        <v>1351</v>
+      </c>
+      <c r="J251" s="5" t="s">
+        <v>1352</v>
+      </c>
+      <c r="K251" s="5" t="n">
+        <v>8899461439</v>
+      </c>
+      <c r="L251" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M251" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N251" s="5" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="O251" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="P251" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q251" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R251" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S251" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T251" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U251" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="1" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B252" s="5" t="n">
+        <v>5947032</v>
+      </c>
+      <c r="C252" s="5" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D252" s="5" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E252" s="5" t="n">
+        <v>9011326474</v>
+      </c>
+      <c r="F252" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="G252" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H252" s="13"/>
+      <c r="I252" s="5" t="s">
+        <v>1358</v>
+      </c>
+      <c r="J252" s="5" t="s">
+        <v>1356</v>
+      </c>
+      <c r="K252" s="5" t="n">
+        <v>9011326474</v>
+      </c>
+      <c r="L252" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="M252" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N252" s="5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O252" s="5"/>
+      <c r="P252" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q252" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R252" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S252" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T252" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U252" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="1" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B253" s="5" t="n">
+        <v>5947046</v>
+      </c>
+      <c r="C253" s="5" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E253" s="5" t="n">
+        <v>7095995117</v>
+      </c>
+      <c r="F253" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G253" s="5" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="H253" s="5" t="s">
+        <v>1362</v>
+      </c>
+      <c r="I253" s="5" t="s">
+        <v>1363</v>
+      </c>
+      <c r="J253" s="5" t="s">
+        <v>1361</v>
+      </c>
+      <c r="K253" s="5" t="n">
+        <v>7095995117</v>
+      </c>
+      <c r="L253" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M253" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N253" s="5" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="O253" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="P253" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q253" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R253" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S253" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T253" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U253" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B254" s="19" t="n">
+        <v>5947047</v>
+      </c>
+      <c r="C254" s="19" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D254" s="19" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E254" s="19" t="n">
+        <v>7776066303</v>
+      </c>
+      <c r="F254" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G254" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H254" s="5" t="s">
+        <v>1367</v>
+      </c>
+      <c r="I254" s="5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="J254" s="5" t="s">
+        <v>1366</v>
+      </c>
+      <c r="K254" s="19" t="n">
+        <v>7776066303</v>
+      </c>
+      <c r="L254" s="5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M254" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N254" s="5" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="O254" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P254" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q254" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R254" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S254" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T254" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U254" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B255" s="19" t="n">
+        <v>5947058</v>
+      </c>
+      <c r="C255" s="19" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D255" s="19" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E255" s="19" t="n">
+        <v>8108484593</v>
+      </c>
+      <c r="F255" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G255" s="5" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="H255" s="5" t="s">
+        <v>1373</v>
+      </c>
+      <c r="I255" s="5" t="s">
+        <v>1374</v>
+      </c>
+      <c r="J255" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="K255" s="19" t="n">
+        <v>8108484593</v>
+      </c>
+      <c r="L255" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="M255" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N255" s="7" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="O255" s="5" t="s">
+        <v>1375</v>
+      </c>
+      <c r="P255" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q255" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R255" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S255" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T255" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U255" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B256" s="5" t="n">
+        <v>5947065</v>
+      </c>
+      <c r="C256" s="5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="D256" s="5" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E256" s="5" t="n">
+        <v>9780945733</v>
+      </c>
+      <c r="F256" s="5" t="s">
+        <v>1379</v>
+      </c>
+      <c r="G256" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H256" s="5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="I256" s="5" t="s">
+        <v>1381</v>
+      </c>
+      <c r="J256" s="5" t="s">
+        <v>1378</v>
+      </c>
+      <c r="K256" s="5" t="n">
+        <v>9780945733</v>
+      </c>
+      <c r="L256" s="5" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M256" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N256" s="5" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="O256" s="5" t="s">
+        <v>1383</v>
+      </c>
+      <c r="P256" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q256" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R256" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S256" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T256" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U256" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B257" s="5" t="n">
+        <v>5947068</v>
+      </c>
+      <c r="C257" s="5" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E257" s="5" t="n">
+        <v>9830505150</v>
+      </c>
+      <c r="F257" s="5" t="s">
+        <v>1387</v>
+      </c>
+      <c r="G257" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H257" s="5" t="s">
+        <v>1388</v>
+      </c>
+      <c r="I257" s="5" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J257" s="5" t="s">
+        <v>1386</v>
+      </c>
+      <c r="K257" s="5" t="n">
+        <v>9830505150</v>
+      </c>
+      <c r="L257" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M257" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N257" s="5" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="O257" s="5" t="s">
+        <v>1389</v>
+      </c>
+      <c r="P257" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q257" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R257" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S257" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T257" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U257" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B258" s="5" t="n">
+        <v>5947074</v>
+      </c>
+      <c r="C258" s="5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D258" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E258" s="5" t="n">
+        <v>9683647822</v>
+      </c>
+      <c r="F258" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G258" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="H258" s="5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I258" s="5" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J258" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="K258" s="5" t="n">
+        <v>9683647822</v>
+      </c>
+      <c r="L258" s="5" t="s">
+        <v>1395</v>
+      </c>
+      <c r="M258" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N258" s="5" t="n">
+        <v>12.11</v>
+      </c>
+      <c r="O258" s="5" t="s">
+        <v>1396</v>
+      </c>
+      <c r="P258" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q258" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R258" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S258" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T258" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U258" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B259" s="5" t="n">
+        <v>5947075</v>
+      </c>
+      <c r="C259" s="5" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D259" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E259" s="5" t="n">
+        <v>9754837577</v>
+      </c>
+      <c r="F259" s="5" t="s">
+        <v>1400</v>
+      </c>
+      <c r="G259" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H259" s="5" t="s">
+        <v>1401</v>
+      </c>
+      <c r="I259" s="5" t="s">
+        <v>1402</v>
+      </c>
+      <c r="J259" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="K259" s="5" t="n">
+        <v>9754837577</v>
+      </c>
+      <c r="L259" s="5" t="s">
+        <v>1400</v>
+      </c>
+      <c r="M259" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N259" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O259" s="5" t="s">
+        <v>1403</v>
+      </c>
+      <c r="P259" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q259" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R259" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S259" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T259" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U259" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B260" s="5" t="n">
+        <v>5947081</v>
+      </c>
+      <c r="C260" s="5" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D260" s="5" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E260" s="5" t="n">
+        <v>9656141422</v>
+      </c>
+      <c r="F260" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G260" s="5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H260" s="5" t="s">
+        <v>1407</v>
+      </c>
+      <c r="I260" s="5" t="s">
+        <v>1405</v>
+      </c>
+      <c r="J260" s="5" t="s">
+        <v>1406</v>
+      </c>
+      <c r="K260" s="5" t="n">
+        <v>9656141422</v>
+      </c>
+      <c r="L260" s="5" t="s">
+        <v>1408</v>
+      </c>
+      <c r="M260" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N260" s="5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="O260" s="5" t="s">
+        <v>1409</v>
+      </c>
+      <c r="P260" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q260" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R260" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S260" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T260" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U260" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B261" s="5" t="n">
+        <v>5947096</v>
+      </c>
+      <c r="C261" s="5" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D261" s="5" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E261" s="5" t="n">
+        <v>9742351067</v>
+      </c>
+      <c r="F261" s="5"/>
+      <c r="G261" s="5" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H261" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I261" s="5" t="s">
+        <v>1411</v>
+      </c>
+      <c r="J261" s="5" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K261" s="5" t="n">
+        <v>9742351067</v>
+      </c>
+      <c r="L261" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M261" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N261" s="5" t="n">
+        <v>6.11</v>
+      </c>
+      <c r="O261" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="P261" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q261" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R261" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S261" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T261" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U261" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="1" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B262" s="5" t="n">
+        <v>5947111</v>
+      </c>
+      <c r="C262" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D262" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E262" s="5" t="n">
+        <v>9690582043</v>
+      </c>
+      <c r="F262" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="G262" s="5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H262" s="5" t="s">
+        <v>1418</v>
+      </c>
+      <c r="I262" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="J262" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="K262" s="5" t="n">
+        <v>9690582043</v>
+      </c>
+      <c r="L262" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="M262" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N262" s="5" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="O262" s="5" t="s">
+        <v>1419</v>
+      </c>
+      <c r="P262" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q262" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R262" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S262" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T262" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U262" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B263" s="5" t="n">
+        <v>5947131</v>
+      </c>
+      <c r="C263" s="5" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D263" s="5" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E263" s="5" t="n">
+        <v>9100231889</v>
+      </c>
+      <c r="F263" s="5"/>
+      <c r="G263" s="5" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="H263" s="5" t="s">
+        <v>1423</v>
+      </c>
+      <c r="I263" s="5" t="s">
+        <v>1421</v>
+      </c>
+      <c r="J263" s="5" t="s">
+        <v>1424</v>
+      </c>
+      <c r="K263" s="5" t="n">
+        <v>9100231889</v>
+      </c>
+      <c r="L263" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M263" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N263" s="5" t="n">
+        <v>8.11</v>
+      </c>
+      <c r="O263" s="5" t="s">
+        <v>1425</v>
+      </c>
+      <c r="P263" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q263" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R263" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S263" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T263" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U263" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B264" s="5" t="n">
+        <v>5947132</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D264" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E264" s="5" t="n">
+        <v>8983580914</v>
+      </c>
+      <c r="F264" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G264" s="5" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="H264" s="5" t="s">
+        <v>1429</v>
+      </c>
+      <c r="I264" s="5" t="s">
+        <v>1427</v>
+      </c>
+      <c r="J264" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K264" s="5" t="n">
+        <v>8983580914</v>
+      </c>
+      <c r="L264" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="M264" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N264" s="5" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="O264" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="P264" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q264" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R264" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S264" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T264" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U264" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B265" s="5" t="n">
+        <v>5947184</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D265" s="5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="E265" s="5" t="n">
+        <v>8838492812</v>
+      </c>
+      <c r="F265" s="5" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G265" s="5" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H265" s="5" t="s">
+        <v>1434</v>
+      </c>
+      <c r="I265" s="5" t="s">
+        <v>1431</v>
+      </c>
+      <c r="J265" s="5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="K265" s="5" t="n">
+        <v>8838492812</v>
+      </c>
+      <c r="L265" s="5" t="s">
+        <v>1433</v>
+      </c>
+      <c r="M265" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N265" s="5" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="O265" s="5" t="s">
+        <v>1435</v>
+      </c>
+      <c r="P265" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q265" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R265" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S265" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T265" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U265" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B266" s="5" t="n">
+        <v>5947190</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D266" s="5" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E266" s="5" t="n">
+        <v>9063226411</v>
+      </c>
+      <c r="F266" s="5"/>
+      <c r="G266" s="5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H266" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I266" s="5" t="s">
+        <v>1437</v>
+      </c>
+      <c r="J266" s="5" t="s">
+        <v>1438</v>
+      </c>
+      <c r="K266" s="5" t="n">
+        <v>9063226411</v>
+      </c>
+      <c r="L266" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M266" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N266" s="5" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="O266" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="P266" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q266" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R266" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S266" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T266" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U266" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="1" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B267" s="5" t="n">
+        <v>5947204</v>
+      </c>
+      <c r="C267" s="5" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D267" s="5" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E267" s="5" t="n">
+        <v>7008537372</v>
+      </c>
+      <c r="F267" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G267" s="5" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="H267" s="5" t="s">
+        <v>1442</v>
+      </c>
+      <c r="I267" s="5" t="s">
+        <v>1443</v>
+      </c>
+      <c r="J267" s="5" t="s">
+        <v>1441</v>
+      </c>
+      <c r="K267" s="5" t="n">
+        <v>7008537372</v>
+      </c>
+      <c r="L267" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M267" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N267" s="5" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="O267" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P267" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q267" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R267" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S267" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T267" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U267" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B268" s="5" t="n">
+        <v>5947211</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D268" s="5" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E268" s="5" t="n">
+        <v>7015517324</v>
+      </c>
+      <c r="F268" s="5" t="s">
+        <v>1447</v>
+      </c>
+      <c r="G268" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H268" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="I268" s="5" t="s">
+        <v>1448</v>
+      </c>
+      <c r="J268" s="5" t="s">
+        <v>1446</v>
+      </c>
+      <c r="K268" s="5" t="n">
+        <v>7015517324</v>
+      </c>
+      <c r="L268" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M268" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N268" s="5" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="O268" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="P268" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q268" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R268" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S268" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T268" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U268" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="1" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B269" s="5" t="n">
+        <v>5947250</v>
+      </c>
+      <c r="C269" s="5" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D269" s="5" t="s">
+        <v>1451</v>
+      </c>
+      <c r="E269" s="5" t="n">
+        <v>9742572959</v>
+      </c>
+      <c r="F269" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G269" s="5" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H269" s="5" t="s">
+        <v>1452</v>
+      </c>
+      <c r="I269" s="5" t="s">
+        <v>1453</v>
+      </c>
+      <c r="J269" s="5" t="s">
+        <v>1451</v>
+      </c>
+      <c r="K269" s="5" t="n">
+        <v>9742572959</v>
+      </c>
+      <c r="L269" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M269" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N269" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O269" s="5" t="s">
+        <v>1454</v>
+      </c>
+      <c r="P269" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q269" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R269" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S269" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T269" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U269" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B270" s="5" t="n">
+        <v>5947259</v>
+      </c>
+      <c r="C270" s="5" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D270" s="5" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E270" s="5" t="n">
+        <v>9591253342</v>
+      </c>
+      <c r="F270" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G270" s="5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H270" s="5" t="s">
+        <v>1458</v>
+      </c>
+      <c r="I270" s="5" t="s">
+        <v>1456</v>
+      </c>
+      <c r="J270" s="5" t="s">
+        <v>1457</v>
+      </c>
+      <c r="K270" s="5" t="n">
+        <v>9591253342</v>
+      </c>
+      <c r="L270" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M270" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N270" s="5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="O270" s="5" t="s">
+        <v>1459</v>
+      </c>
+      <c r="P270" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q270" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R270" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S270" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T270" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U270" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B271" s="5" t="n">
+        <v>5947272</v>
+      </c>
+      <c r="C271" s="5" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D271" s="5" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E271" s="5" t="n">
+        <v>9448213688</v>
+      </c>
+      <c r="F271" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="G271" s="5" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="H271" s="5" t="s">
+        <v>1463</v>
+      </c>
+      <c r="I271" s="5" t="s">
+        <v>1461</v>
+      </c>
+      <c r="J271" s="5" t="s">
+        <v>1462</v>
+      </c>
+      <c r="K271" s="5" t="n">
+        <v>9448213688</v>
+      </c>
+      <c r="L271" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M271" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N271" s="5" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="O271" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P271" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q271" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R271" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S271" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T271" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U271" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B272" s="5" t="n">
+        <v>5947293</v>
+      </c>
+      <c r="C272" s="5" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D272" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E272" s="5" t="n">
+        <v>8903150289</v>
+      </c>
+      <c r="F272" s="5" t="s">
+        <v>1467</v>
+      </c>
+      <c r="G272" s="5" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="H272" s="5"/>
+      <c r="I272" s="5" t="s">
+        <v>1465</v>
+      </c>
+      <c r="J272" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="K272" s="5" t="n">
+        <v>8903150289</v>
+      </c>
+      <c r="L272" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M272" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N272" s="5" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="O272" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="P272" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q272" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R272" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S272" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T272" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U272" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B273" s="5" t="n">
+        <v>5947294</v>
+      </c>
+      <c r="C273" s="5" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D273" s="5" t="s">
+        <v>1470</v>
+      </c>
+      <c r="E273" s="5" t="n">
+        <v>7339124359</v>
+      </c>
+      <c r="F273" s="5" t="s">
+        <v>1471</v>
+      </c>
+      <c r="G273" s="5" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H273" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="I273" s="5" t="s">
+        <v>1469</v>
+      </c>
+      <c r="J273" s="5" t="s">
+        <v>1470</v>
+      </c>
+      <c r="K273" s="5" t="n">
+        <v>7339124359</v>
+      </c>
+      <c r="L273" s="5" t="s">
+        <v>1471</v>
+      </c>
+      <c r="M273" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N273" s="5" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="O273" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="P273" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q273" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R273" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S273" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T273" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U273" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B274" s="5" t="n">
+        <v>5947326</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D274" s="5" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E274" s="5" t="n">
+        <v>8932030362</v>
+      </c>
+      <c r="F274" s="5"/>
+      <c r="G274" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H274" s="5" t="s">
+        <v>1476</v>
+      </c>
+      <c r="I274" s="5" t="s">
+        <v>1474</v>
+      </c>
+      <c r="J274" s="5" t="s">
+        <v>1475</v>
+      </c>
+      <c r="K274" s="5" t="n">
+        <v>8932030362</v>
+      </c>
+      <c r="L274" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M274" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N274" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O274" s="5" t="s">
+        <v>1476</v>
+      </c>
+      <c r="P274" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q274" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R274" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S274" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T274" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U274" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B275" s="5" t="n">
+        <v>5947327</v>
+      </c>
+      <c r="C275" s="5" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D275" s="5" t="s">
+        <v>1479</v>
+      </c>
+      <c r="E275" s="5" t="n">
+        <v>8103916415</v>
+      </c>
+      <c r="F275" s="5" t="s">
+        <v>1480</v>
+      </c>
+      <c r="G275" s="5" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="H275" s="5" t="s">
+        <v>1481</v>
+      </c>
+      <c r="I275" s="5" t="s">
+        <v>1482</v>
+      </c>
+      <c r="J275" s="5" t="s">
+        <v>1479</v>
+      </c>
+      <c r="K275" s="5" t="n">
+        <v>8103916415</v>
+      </c>
+      <c r="L275" s="5" t="s">
+        <v>1480</v>
+      </c>
+      <c r="M275" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N275" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O275" s="5" t="s">
+        <v>1483</v>
+      </c>
+      <c r="P275" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q275" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R275" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S275" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T275" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U275" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B276" s="5" t="n">
+        <v>5947328</v>
+      </c>
+      <c r="C276" s="5" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D276" s="5" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E276" s="5" t="n">
+        <v>9118778428</v>
+      </c>
+      <c r="F276" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G276" s="5" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H276" s="5" t="s">
+        <v>1487</v>
+      </c>
+      <c r="I276" s="5" t="s">
+        <v>1488</v>
+      </c>
+      <c r="J276" s="5" t="s">
+        <v>1486</v>
+      </c>
+      <c r="K276" s="5" t="n">
+        <v>9118778428</v>
+      </c>
+      <c r="L276" s="5" t="s">
+        <v>1489</v>
+      </c>
+      <c r="M276" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N276" s="8" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="O276" s="5" t="s">
+        <v>1490</v>
+      </c>
+      <c r="P276" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q276" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R276" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S276" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T276" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U276" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B277" s="5" t="n">
+        <v>5947329</v>
+      </c>
+      <c r="C277" s="5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D277" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="E277" s="5" t="n">
+        <v>9392083881</v>
+      </c>
+      <c r="F277" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G277" s="5" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="H277" s="5" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I277" s="5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="J277" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="K277" s="5" t="n">
+        <v>9392083881</v>
+      </c>
+      <c r="L277" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M277" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N277" s="5" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="O277" s="5" t="s">
+        <v>1495</v>
+      </c>
+      <c r="P277" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q277" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R277" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S277" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T277" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U277" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B278" s="5" t="n">
+        <v>5950026</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D278" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="E278" s="5" t="n">
+        <v>8522871339</v>
+      </c>
+      <c r="F278" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="G278" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H278" s="5"/>
+      <c r="I278" s="5" t="s">
+        <v>1499</v>
+      </c>
+      <c r="J278" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="K278" s="5" t="n">
+        <v>8522871339</v>
+      </c>
+      <c r="L278" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M278" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N278" s="5" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="O278" s="5" t="s">
+        <v>1500</v>
+      </c>
+      <c r="P278" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q278" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R278" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S278" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T278" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U278" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B279" s="5" t="n">
+        <v>5947352</v>
+      </c>
+      <c r="C279" s="5" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D279" s="5" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E279" s="5" t="n">
+        <v>9682931298</v>
+      </c>
+      <c r="F279" s="5" t="s">
+        <v>1504</v>
+      </c>
+      <c r="G279" s="5" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="H279" s="5" t="s">
+        <v>1505</v>
+      </c>
+      <c r="I279" s="5" t="s">
+        <v>1502</v>
+      </c>
+      <c r="J279" s="5" t="s">
+        <v>1503</v>
+      </c>
+      <c r="K279" s="5" t="n">
+        <v>9682931298</v>
+      </c>
+      <c r="L279" s="5" t="s">
+        <v>1504</v>
+      </c>
+      <c r="M279" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N279" s="7" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="O279" s="5" t="s">
+        <v>1506</v>
+      </c>
+      <c r="P279" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q279" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R279" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S279" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T279" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U279" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B280" s="5" t="n">
+        <v>5947353</v>
+      </c>
+      <c r="C280" s="5" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D280" s="5" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E280" s="5" t="n">
+        <v>9920883640</v>
+      </c>
+      <c r="F280" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G280" s="5" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="H280" s="5" t="s">
+        <v>1510</v>
+      </c>
+      <c r="I280" s="5" t="s">
+        <v>1508</v>
+      </c>
+      <c r="J280" s="5" t="s">
+        <v>1509</v>
+      </c>
+      <c r="K280" s="5" t="n">
+        <v>9920883640</v>
+      </c>
+      <c r="L280" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="M280" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N280" s="5" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="O280" s="5" t="s">
+        <v>1511</v>
+      </c>
+      <c r="P280" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q280" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R280" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S280" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T280" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U280" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B281" s="5" t="n">
+        <v>5947371</v>
+      </c>
+      <c r="C281" s="5" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D281" s="5" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E281" s="5" t="n">
+        <v>9828056080</v>
+      </c>
+      <c r="F281" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G281" s="5" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H281" s="5" t="s">
+        <v>1515</v>
+      </c>
+      <c r="I281" s="5" t="s">
+        <v>1513</v>
+      </c>
+      <c r="J281" s="5" t="s">
+        <v>1516</v>
+      </c>
+      <c r="K281" s="5" t="n">
+        <v>9828056080</v>
+      </c>
+      <c r="L281" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="M281" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N281" s="5" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="O281" s="5" t="s">
+        <v>1517</v>
+      </c>
+      <c r="P281" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q281" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R281" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S281" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T281" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U281" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="1" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B282" s="5" t="n">
+        <v>5947393</v>
+      </c>
+      <c r="C282" s="5" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D282" s="5" t="s">
+        <v>1520</v>
+      </c>
+      <c r="E282" s="5" t="n">
+        <v>8108320207</v>
+      </c>
+      <c r="F282" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G282" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="H282" s="5" t="s">
+        <v>1521</v>
+      </c>
+      <c r="I282" s="5" t="s">
+        <v>1519</v>
+      </c>
+      <c r="J282" s="5" t="s">
+        <v>1520</v>
+      </c>
+      <c r="K282" s="5" t="n">
+        <v>8108320207</v>
+      </c>
+      <c r="L282" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="M282" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N282" s="8" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="O282" s="5" t="s">
+        <v>1521</v>
+      </c>
+      <c r="P282" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q282" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R282" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S282" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T282" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U282" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B283" s="5" t="n">
+        <v>5947411</v>
+      </c>
+      <c r="C283" s="5" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D283" s="5" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E283" s="5" t="n">
+        <v>8050347903</v>
+      </c>
+      <c r="F283" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G283" s="5" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="H283" s="5" t="s">
+        <v>1525</v>
+      </c>
+      <c r="I283" s="5" t="s">
+        <v>1523</v>
+      </c>
+      <c r="J283" s="5" t="s">
+        <v>1524</v>
+      </c>
+      <c r="K283" s="5" t="n">
+        <v>8050347903</v>
+      </c>
+      <c r="L283" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M283" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N283" s="8" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="O283" s="20" t="s">
+        <v>1526</v>
+      </c>
+      <c r="P283" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q283" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R283" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S283" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T283" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U283" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="1" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B284" s="5" t="n">
+        <v>5947432</v>
+      </c>
+      <c r="C284" s="5" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D284" s="5" t="s">
+        <v>1529</v>
+      </c>
+      <c r="E284" s="5" t="n">
+        <v>9672897025</v>
+      </c>
+      <c r="F284" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G284" s="5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H284" s="5" t="s">
+        <v>1530</v>
+      </c>
+      <c r="I284" s="5" t="s">
+        <v>1528</v>
+      </c>
+      <c r="J284" s="5" t="s">
+        <v>1529</v>
+      </c>
+      <c r="K284" s="5" t="n">
+        <v>9761603139</v>
+      </c>
+      <c r="L284" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M284" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N284" s="5" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="O284" s="5" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P284" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q284" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R284" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S284" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T284" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U284" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="1" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B285" s="5" t="n">
+        <v>5947482</v>
+      </c>
+      <c r="C285" s="5" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D285" s="5" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E285" s="5" t="n">
+        <v>8788856590</v>
+      </c>
+      <c r="F285" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G285" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="H285" s="5" t="s">
+        <v>1535</v>
+      </c>
+      <c r="I285" s="5" t="s">
+        <v>1533</v>
+      </c>
+      <c r="J285" s="5" t="s">
+        <v>1534</v>
+      </c>
+      <c r="K285" s="5" t="n">
+        <v>8788856590</v>
+      </c>
+      <c r="L285" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="M285" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N285" s="8" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="O285" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P285" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q285" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R285" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S285" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T285" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U285" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="1" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B286" s="19" t="n">
+        <v>5947502</v>
+      </c>
+      <c r="C286" s="19" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D286" s="19" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E286" s="5" t="n">
+        <v>9711448744</v>
+      </c>
+      <c r="F286" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="G286" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H286" s="5" t="s">
+        <v>1539</v>
+      </c>
+      <c r="I286" s="19" t="s">
+        <v>1537</v>
+      </c>
+      <c r="J286" s="19" t="s">
+        <v>1538</v>
+      </c>
+      <c r="K286" s="5" t="n">
+        <v>9711448744</v>
+      </c>
+      <c r="L286" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M286" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="N286" s="5" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="O286" s="5" t="s">
+        <v>1540</v>
+      </c>
+      <c r="P286" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q286" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R286" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S286" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T286" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U286" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B287" s="5" t="n">
+        <v>5947505</v>
+      </c>
+      <c r="C287" s="5" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D287" s="5" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E287" s="5" t="n">
+        <v>9962466624</v>
+      </c>
+      <c r="F287" s="5"/>
+      <c r="G287" s="5" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="H287" s="5" t="s">
+        <v>1544</v>
+      </c>
+      <c r="I287" s="5" t="s">
+        <v>1542</v>
+      </c>
+      <c r="J287" s="5" t="s">
+        <v>1543</v>
+      </c>
+      <c r="K287" s="5" t="n">
+        <v>9962466624</v>
+      </c>
+      <c r="L287" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="M287" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="N287" s="5" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="O287" s="5" t="s">
+        <v>1545</v>
+      </c>
+      <c r="P287" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q287" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R287" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S287" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T287" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U287" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -19493,7 +23454,7 @@
       <formula>NOT(ISERROR(SEARCH("Acceptable",T56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T95:T101 T93 T88 T87 T85 T82 T77 T75 T72 T69:T70 T65:T67 T58 T152:T238">
+  <conditionalFormatting sqref="T95:T101 T93 T88 T87 T85 T82 T77 T75 T72 T69:T70 T65:T67 T58 T152:T287">
     <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Acceptable" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("Acceptable",T58)))</formula>
     </cfRule>
@@ -19537,7 +23498,15 @@
       <formula>NOT(ISERROR(SEARCH("No Change",P199)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="13">
+  <conditionalFormatting sqref="P239:U287">
+    <cfRule type="containsText" priority="28" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="No Change" dxfId="2">
+      <formula>NOT(ISERROR(SEARCH("No Change",P239)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="29" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Change" dxfId="1">
+      <formula>NOT(ISERROR(SEARCH("Change",P239)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="15">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:U3 P4:S11 U4:U6 T5" type="list">
       <formula1>"Change,No Change"</formula1>
       <formula2>0</formula2>
@@ -19590,6 +23559,14 @@
       <formula1>"Change,No Change,Acceptable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P239:S287 U239:U287" type="list">
+      <formula1>"Change,No Change"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T239:T287" type="list">
+      <formula1>"Change,No Change,Acceptable"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="J110" r:id="rId1" display="kovuru@hotmail.com"/>

</xml_diff>